<commit_message>
feat: adicionando descrição de pib per capita
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Renan\Arquivos-da-Universidade\8_PERIODO\SISTEMA_DE_APOIO_DE_DADOS\projeto_sad\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Renan\Arquivos-da-Universidade\8_PERIODO\SISTEMA_DE_APOIO_DE_DADOS\projeto_sad\projeto_producao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13A4648-3C24-4AA7-AA92-D836429BCEBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EB48D1-AC0F-4D05-B553-FDC7B7F96662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{6EF6CF19-DB0D-4222-8BAB-A21ADA3254A6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Variável</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>Nome da região geográfica (Ex: Nordeste)</t>
+  </si>
+  <si>
+    <t>pib per capita</t>
+  </si>
+  <si>
+    <t>Média da riqueza produzida por cada habitante de um município em determinado período, geralmente um ano.</t>
   </si>
 </sst>
 </file>
@@ -186,7 +192,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -203,11 +209,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="5">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -215,7 +227,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -236,9 +248,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -253,12 +262,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2AAF961D-A2CB-411B-975C-3010E9888CAD}" name="Tabela1" displayName="Tabela1" ref="A1:C14" totalsRowShown="0" headerRowDxfId="3" dataDxfId="4">
-  <autoFilter ref="A1:C14" xr:uid="{2AAF961D-A2CB-411B-975C-3010E9888CAD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{2AAF961D-A2CB-411B-975C-3010E9888CAD}" name="Tabela1" displayName="Tabela1" ref="A1:C15" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C15" xr:uid="{2AAF961D-A2CB-411B-975C-3010E9888CAD}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{E78D585C-67CC-4A62-AD5E-9604C84536EA}" name="Variável" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{E78D585C-67CC-4A62-AD5E-9604C84536EA}" name="Variável" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{C22B843A-FEE2-4DC7-AC4E-2A58A8EC00F4}" name="Tipo" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{B3927394-2DFD-4403-8DE8-97522DDB5A40}" name="Descrição" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B3927394-2DFD-4403-8DE8-97522DDB5A40}" name="Descrição" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -581,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69B49887-4386-47BC-A788-C00496C0862F}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +603,7 @@
     <col min="3" max="3" width="65.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -616,136 +625,147 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="D7" s="1"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: fixing file path
</commit_message>
<xml_diff>
--- a/metadata.xlsx
+++ b/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Renan\Arquivos-da-Universidade\8_PERIODO\SISTEMA_DE_APOIO_DE_DADOS\projeto_sad\projeto_producao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Renan\Arquivos-da-Universidade\8_PERIODO\SISTEMA_DE_APOIO_A_DECISSAO\projeto_sad\projeto_producao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8EB48D1-AC0F-4D05-B553-FDC7B7F96662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36AFA3C6-93A8-4466-AD4F-EEC61CCA7BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{6EF6CF19-DB0D-4222-8BAB-A21ADA3254A6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{6EF6CF19-DB0D-4222-8BAB-A21ADA3254A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -593,7 +593,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>